<commit_message>
specSpring4RestTomcat is working; refactoring
</commit_message>
<xml_diff>
--- a/doc/classes.xlsx
+++ b/doc/classes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karlcoka\eclipse_workspace\ws_sandbox\jump\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\jump\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>spec</t>
   </si>
@@ -108,6 +108,24 @@
   </si>
   <si>
     <t>Tomcat, servlet3Support</t>
+  </si>
+  <si>
+    <t>webappFirst</t>
+  </si>
+  <si>
+    <t>Tomcat, UserResource</t>
+  </si>
+  <si>
+    <t>webappAngular</t>
+  </si>
+  <si>
+    <t>Wildfly, UserResource, tutti, war</t>
+  </si>
+  <si>
+    <t>buildAppSimpleSpring</t>
+  </si>
+  <si>
+    <t>+</t>
   </si>
 </sst>
 </file>
@@ -502,9 +520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -588,73 +604,121 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
     <col min="5" max="5" width="28.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="7" max="7" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
       </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E5">
+    <sortCondition ref="A2:A5"/>
+    <sortCondition ref="B2:B5"/>
+    <sortCondition ref="C2:C5"/>
+    <sortCondition ref="D2:D5"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
spring4RestWildfly added; spring4RestTomcat produces JSON
</commit_message>
<xml_diff>
--- a/doc/classes.xlsx
+++ b/doc/classes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>spec</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>+</t>
+  </si>
+  <si>
+    <t>spring4RestWildfly</t>
+  </si>
+  <si>
+    <t>Wildfly, servlet3Support</t>
   </si>
 </sst>
 </file>
@@ -604,11 +610,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -689,10 +693,16 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -706,18 +716,35 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E5">
-    <sortCondition ref="A2:A5"/>
-    <sortCondition ref="B2:B5"/>
-    <sortCondition ref="C2:C5"/>
-    <sortCondition ref="D2:D5"/>
+  <sortState ref="A2:G6">
+    <sortCondition ref="A2:A6"/>
+    <sortCondition ref="B2:B6"/>
+    <sortCondition ref="C2:C6"/>
+    <sortCondition ref="D2:D6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
WebFramework attribute added; appGeneration method with reflection
</commit_message>
<xml_diff>
--- a/doc/classes.xlsx
+++ b/doc/classes.xlsx
@@ -15,6 +15,9 @@
     <sheet name="classes" sheetId="1" r:id="rId1"/>
     <sheet name="samples" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">samples!$A$1:$D$7</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>spec</t>
   </si>
@@ -92,9 +95,6 @@
     <t>PredefinedAngularAppBuilder</t>
   </si>
   <si>
-    <t>StandaloneAngularGenerator</t>
-  </si>
-  <si>
     <t>browser</t>
   </si>
   <si>
@@ -107,31 +107,43 @@
     <t>PredefinedWebAppBuilder</t>
   </si>
   <si>
-    <t>Tomcat, servlet3Support</t>
-  </si>
-  <si>
     <t>webappFirst</t>
   </si>
   <si>
     <t>webappAngular</t>
   </si>
   <si>
-    <t>Wildfly, UserResource, tutti, war</t>
-  </si>
-  <si>
     <t>buildAppSimpleSpring</t>
   </si>
   <si>
-    <t>+</t>
-  </si>
-  <si>
     <t>spring4RestWildfly</t>
   </si>
   <si>
-    <t>Wildfly, servlet3Support</t>
-  </si>
-  <si>
-    <t>Tomcat, UserResource, web.xml</t>
+    <t>webappSimple</t>
+  </si>
+  <si>
+    <t>targetContainer</t>
+  </si>
+  <si>
+    <t>TOMCAT</t>
+  </si>
+  <si>
+    <t>WILDFLY</t>
+  </si>
+  <si>
+    <t>servlet3Support</t>
+  </si>
+  <si>
+    <t>UserResource, tutti, war</t>
+  </si>
+  <si>
+    <t>UserResource, web.xml</t>
+  </si>
+  <si>
+    <t>buildAppSimple</t>
+  </si>
+  <si>
+    <t>(inline)</t>
   </si>
 </sst>
 </file>
@@ -610,141 +622,131 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
     <col min="5" max="5" width="28.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="7" max="7" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
         <v>33</v>
       </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G6">
+  <autoFilter ref="A1:D7"/>
+  <sortState ref="A2:D6">
     <sortCondition ref="A2:A6"/>
     <sortCondition ref="B2:B6"/>
-    <sortCondition ref="C2:C6"/>
-    <sortCondition ref="D2:D6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>